<commit_message>
update xls and add test about json to GAS
</commit_message>
<xml_diff>
--- a/template/PLAN.xlsx
+++ b/template/PLAN.xlsx
@@ -17,76 +17,103 @@
     <sheet name="概要表" sheetId="3" r:id="rId3"/>
     <sheet name="位置圖" sheetId="4" r:id="rId4"/>
     <sheet name="輸水損失改善" sheetId="5" r:id="rId5"/>
+    <sheet name="簡報" sheetId="6" r:id="rId6"/>
   </sheets>
+  <externalReferences>
+    <externalReference r:id="rId7"/>
+  </externalReferences>
   <definedNames>
+    <definedName name="_1¨F¤l³æ_ù" localSheetId="5">#REF!</definedName>
     <definedName name="_1¨F¤l³æ_ù">#REF!</definedName>
+    <definedName name="_5·s_WºÙ" localSheetId="5" hidden="1">#REF!</definedName>
     <definedName name="_5·s_WºÙ" hidden="1">#REF!</definedName>
     <definedName name="_Fill" localSheetId="3">#REF!</definedName>
     <definedName name="_Fill" localSheetId="2">#REF!</definedName>
+    <definedName name="_Fill" localSheetId="5">#REF!</definedName>
     <definedName name="_Fill">#REF!</definedName>
     <definedName name="aaaa" localSheetId="3">#REF!</definedName>
     <definedName name="aaaa" localSheetId="2">#REF!</definedName>
+    <definedName name="aaaa" localSheetId="5">#REF!</definedName>
     <definedName name="aaaa">#REF!</definedName>
     <definedName name="j" localSheetId="3">#REF!</definedName>
     <definedName name="j" localSheetId="2">#REF!</definedName>
+    <definedName name="j" localSheetId="5">#REF!</definedName>
     <definedName name="j">#REF!</definedName>
     <definedName name="k" localSheetId="3">#REF!</definedName>
     <definedName name="k" localSheetId="2">#REF!</definedName>
+    <definedName name="k" localSheetId="5">#REF!</definedName>
     <definedName name="k">#REF!</definedName>
     <definedName name="m" localSheetId="3">#REF!</definedName>
     <definedName name="m" localSheetId="2">#REF!</definedName>
+    <definedName name="m" localSheetId="5">#REF!</definedName>
     <definedName name="m">#REF!</definedName>
     <definedName name="ppp" localSheetId="3">#REF!</definedName>
     <definedName name="ppp" localSheetId="2">#REF!</definedName>
+    <definedName name="ppp" localSheetId="5">#REF!</definedName>
     <definedName name="ppp">#REF!</definedName>
     <definedName name="_xlnm.Print_Area" localSheetId="2">概要表!$A$1:$M$22</definedName>
     <definedName name="小給11數量計算" localSheetId="3">#REF!</definedName>
     <definedName name="小給11數量計算" localSheetId="2">#REF!</definedName>
     <definedName name="小給11數量計算" localSheetId="4" hidden="1">#REF!</definedName>
+    <definedName name="小給11數量計算" localSheetId="5">#REF!</definedName>
     <definedName name="小給11數量計算">#REF!</definedName>
     <definedName name="水隊" localSheetId="3">#REF!</definedName>
     <definedName name="水隊" localSheetId="2">#REF!</definedName>
     <definedName name="水隊" localSheetId="4" hidden="1">#REF!</definedName>
+    <definedName name="水隊" localSheetId="5">#REF!</definedName>
     <definedName name="水隊">#REF!</definedName>
     <definedName name="水隊小給11數量計算表" localSheetId="3">#REF!</definedName>
     <definedName name="水隊小給11數量計算表" localSheetId="2">#REF!</definedName>
+    <definedName name="水隊小給11數量計算表" localSheetId="5">#REF!</definedName>
     <definedName name="水隊小給11數量計算表">#REF!</definedName>
     <definedName name="石" localSheetId="3">#REF!</definedName>
     <definedName name="石" localSheetId="2">#REF!</definedName>
+    <definedName name="石" localSheetId="5">#REF!</definedName>
     <definedName name="石">#REF!</definedName>
     <definedName name="沙" localSheetId="3">#REF!</definedName>
     <definedName name="沙" localSheetId="2">#REF!</definedName>
+    <definedName name="沙" localSheetId="5">#REF!</definedName>
     <definedName name="沙">#REF!</definedName>
     <definedName name="初稿審核單1" localSheetId="3">#REF!</definedName>
     <definedName name="初稿審核單1" localSheetId="2">#REF!</definedName>
+    <definedName name="初稿審核單1" localSheetId="5">#REF!</definedName>
     <definedName name="初稿審核單1">#REF!</definedName>
     <definedName name="洗沙子單價" localSheetId="3">#REF!</definedName>
     <definedName name="洗沙子單價" localSheetId="2">#REF!</definedName>
     <definedName name="洗沙子單價" localSheetId="4">#REF!</definedName>
+    <definedName name="洗沙子單價" localSheetId="5">#REF!</definedName>
     <definedName name="洗沙子單價">#REF!</definedName>
     <definedName name="計劃說明1" localSheetId="3">#REF!</definedName>
     <definedName name="計劃說明1" localSheetId="2">#REF!</definedName>
+    <definedName name="計劃說明1" localSheetId="5">#REF!</definedName>
     <definedName name="計劃說明1">#REF!</definedName>
     <definedName name="幹線" localSheetId="3">#REF!</definedName>
     <definedName name="幹線" localSheetId="2">#REF!</definedName>
+    <definedName name="幹線" localSheetId="5">#REF!</definedName>
     <definedName name="幹線">#REF!</definedName>
     <definedName name="新名稱" localSheetId="3">#REF!</definedName>
     <definedName name="新名稱" localSheetId="2">#REF!</definedName>
+    <definedName name="新名稱" localSheetId="5">#REF!</definedName>
     <definedName name="新名稱">#REF!</definedName>
     <definedName name="溪" localSheetId="3">#REF!</definedName>
     <definedName name="溪" localSheetId="2">#REF!</definedName>
+    <definedName name="溪" localSheetId="5">#REF!</definedName>
     <definedName name="溪">#REF!</definedName>
     <definedName name="溪心" localSheetId="3">#REF!</definedName>
     <definedName name="溪心" localSheetId="2">#REF!</definedName>
+    <definedName name="溪心" localSheetId="5">#REF!</definedName>
     <definedName name="溪心">#REF!</definedName>
     <definedName name="預算" localSheetId="3">#REF!</definedName>
     <definedName name="預算" localSheetId="2">#REF!</definedName>
+    <definedName name="預算" localSheetId="5">#REF!</definedName>
     <definedName name="預算">#REF!</definedName>
     <definedName name="頭" localSheetId="3">#REF!</definedName>
     <definedName name="頭" localSheetId="2">#REF!</definedName>
+    <definedName name="頭" localSheetId="5">#REF!</definedName>
     <definedName name="頭">#REF!</definedName>
     <definedName name="蘆北支線3" localSheetId="3">#REF!</definedName>
     <definedName name="蘆北支線3" localSheetId="2">#REF!</definedName>
+    <definedName name="蘆北支線3" localSheetId="5">#REF!</definedName>
     <definedName name="蘆北支線3">#REF!</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
@@ -460,7 +487,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="117">
   <si>
     <t xml:space="preserve">農田水利設施更新改善工程-提報明細表       </t>
   </si>
@@ -837,6 +864,188 @@
   </si>
   <si>
     <t>施工簡圖</t>
+    <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>工程內容：U型溝、改善長度</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>750</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>公尺、</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">          設計斷面</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>渠寬</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>0.8</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>M</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>*</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="20"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>渠高</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>0.7</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FF000000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t>M</t>
+    </r>
+  </si>
+  <si>
+    <t>現況概述：本線為72年新生重劃,現況為內面</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          工斷面，破損嚴重，影響排水機</t>
+  </si>
+  <si>
+    <t>改善位置圖</t>
+  </si>
+  <si>
+    <t>現地照片</t>
+  </si>
+  <si>
+    <t>OOOO改善工程</t>
+    <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>工作站別：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t/>
+    </r>
+    <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <t>工程地點：</t>
+    <phoneticPr fontId="24" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>概估經費：</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="54"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="標楷體"/>
+        <family val="4"/>
+        <charset val="136"/>
+      </rPr>
+      <t/>
+    </r>
     <phoneticPr fontId="24" type="noConversion"/>
   </si>
 </sst>
@@ -854,7 +1063,7 @@
     <numFmt numFmtId="182" formatCode="#,###&quot;元&quot;"/>
     <numFmt numFmtId="183" formatCode="0.000"/>
   </numFmts>
-  <fonts count="38">
+  <fonts count="45">
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
@@ -1098,6 +1307,54 @@
       <color rgb="FFFF0000"/>
       <name val="PMingLiu"/>
       <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="70"/>
+      <color rgb="FF000000"/>
+      <name val="PMingLiu"/>
+      <family val="1"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="70"/>
+      <color rgb="FF000000"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="54"/>
+      <color rgb="FF000000"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="54"/>
+      <color rgb="FFFF0000"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="20"/>
+      <color rgb="FF000000"/>
+      <name val="標楷體"/>
+      <family val="4"/>
+      <charset val="136"/>
+    </font>
+    <font>
+      <sz val="40"/>
+      <color rgb="FF000000"/>
+      <name val="標楷體"/>
+      <family val="4"/>
       <charset val="136"/>
     </font>
   </fonts>
@@ -1580,11 +1837,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="8"/>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="8"/>
   </cellStyleXfs>
-  <cellXfs count="152">
+  <cellXfs count="161">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1818,6 +2076,8 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1848,6 +2108,43 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment shrinkToFit="1"/>
+    </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -1860,13 +2157,6 @@
     <xf numFmtId="180" fontId="16" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1887,9 +2177,6 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1935,33 +2222,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1973,12 +2233,36 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="0" borderId="8" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="5"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="41" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="0" borderId="8" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="一般" xfId="0" builtinId="0"/>
     <cellStyle name="一般 2" xfId="1"/>
+    <cellStyle name="一般 3" xfId="2"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -2013,7 +2297,7 @@
         <xdr:cNvPr id="2" name="圖片 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{436E7E13-ED1D-47C0-A9BF-B34C71C5D5BC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{436E7E13-ED1D-47C0-A9BF-B34C71C5D5BC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2057,7 +2341,7 @@
         <xdr:cNvPr id="5" name="AutoShape 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2155,7 +2439,7 @@
         <xdr:cNvPr id="6" name="Line 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2207,7 +2491,7 @@
         <xdr:cNvPr id="3" name="圖片 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C0C361B7-C47F-404F-A700-CEF5FB854306}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{C0C361B7-C47F-404F-A700-CEF5FB854306}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2251,7 +2535,7 @@
         <xdr:cNvPr id="4" name="圖片 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01B38F41-0753-4957-93B7-822BBB8BB3CA}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{01B38F41-0753-4957-93B7-822BBB8BB3CA}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2295,7 +2579,7 @@
         <xdr:cNvPr id="5" name="矩形 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{B90EFD2D-F368-486E-B0BF-3201274FFD30}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{B90EFD2D-F368-486E-B0BF-3201274FFD30}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2345,6 +2629,187 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>276225</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>99060</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="矩形 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="276225" y="11049000"/>
+          <a:ext cx="13134975" cy="7195185"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>571500</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>66675</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="矩形 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="571500" y="21002625"/>
+          <a:ext cx="5972175" cy="7505700"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>55</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>89</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="矩形 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7181850" y="20974050"/>
+          <a:ext cx="6057900" cy="7553325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:sysClr val="windowText" lastClr="000000"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr rot="0" spcFirstLastPara="0" vert="horz" wrap="square" lIns="91440" tIns="45720" rIns="91440" bIns="45720" numCol="1" spcCol="0" rtlCol="0" fromWordArt="0" anchor="ctr" anchorCtr="0" forceAA="0" compatLnSpc="1">
+          <a:prstTxWarp prst="textNoShape">
+            <a:avLst/>
+          </a:prstTxWarp>
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="zh-TW" altLang="en-US"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
+    <sheetNames>
+      <sheetName val="封面"/>
+      <sheetName val="提報明細表"/>
+      <sheetName val="概要表"/>
+      <sheetName val="位置圖"/>
+      <sheetName val="輸水損失改善"/>
+      <sheetName val="簡報"/>
+    </sheetNames>
+    <sheetDataSet>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+    </sheetDataSet>
+  </externalBook>
+</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2722,28 +3187,28 @@
       <c r="I1" s="1"/>
     </row>
     <row r="2" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A2" s="85" t="s">
+      <c r="A2" s="87" t="s">
         <v>102</v>
       </c>
-      <c r="B2" s="85"/>
-      <c r="C2" s="85"/>
-      <c r="D2" s="85"/>
-      <c r="E2" s="85"/>
-      <c r="F2" s="85"/>
-      <c r="G2" s="85"/>
-      <c r="H2" s="85"/>
-      <c r="I2" s="85"/>
+      <c r="B2" s="87"/>
+      <c r="C2" s="87"/>
+      <c r="D2" s="87"/>
+      <c r="E2" s="87"/>
+      <c r="F2" s="87"/>
+      <c r="G2" s="87"/>
+      <c r="H2" s="87"/>
+      <c r="I2" s="87"/>
     </row>
     <row r="3" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A3" s="85"/>
-      <c r="B3" s="85"/>
-      <c r="C3" s="85"/>
-      <c r="D3" s="85"/>
-      <c r="E3" s="85"/>
-      <c r="F3" s="85"/>
-      <c r="G3" s="85"/>
-      <c r="H3" s="85"/>
-      <c r="I3" s="85"/>
+      <c r="A3" s="87"/>
+      <c r="B3" s="87"/>
+      <c r="C3" s="87"/>
+      <c r="D3" s="87"/>
+      <c r="E3" s="87"/>
+      <c r="F3" s="87"/>
+      <c r="G3" s="87"/>
+      <c r="H3" s="87"/>
+      <c r="I3" s="87"/>
     </row>
     <row r="4" spans="1:9" ht="16.5" customHeight="1">
       <c r="A4" s="1"/>
@@ -2790,17 +3255,17 @@
       <c r="I7" s="1"/>
     </row>
     <row r="8" spans="1:9" ht="40.5" customHeight="1">
-      <c r="A8" s="86" t="s">
+      <c r="A8" s="88" t="s">
         <v>104</v>
       </c>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
     </row>
     <row r="9" spans="1:9" ht="16.5" customHeight="1">
       <c r="A9" s="1"/>
@@ -2836,15 +3301,15 @@
       <c r="I11" s="1"/>
     </row>
     <row r="12" spans="1:9" ht="16.5" customHeight="1">
-      <c r="A12" s="83"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
+      <c r="A12" s="85"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
     </row>
     <row r="13" spans="1:9" ht="16.5" customHeight="1">
       <c r="A13" s="3"/>
@@ -2858,28 +3323,28 @@
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" ht="129" customHeight="1">
-      <c r="A14" s="83"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="84"/>
+      <c r="A14" s="85"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
     </row>
     <row r="15" spans="1:9" ht="28.9" customHeight="1">
-      <c r="A15" s="85" t="s">
+      <c r="A15" s="87" t="s">
         <v>103</v>
       </c>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
     </row>
     <row r="16" spans="1:9" ht="16.5" customHeight="1"/>
     <row r="17" ht="16.5" customHeight="1"/>
@@ -3017,18 +3482,18 @@
       <c r="L1" s="6"/>
     </row>
     <row r="2" spans="1:12" ht="27.75" customHeight="1">
-      <c r="A2" s="88" t="s">
+      <c r="A2" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="84"/>
-      <c r="C2" s="84"/>
-      <c r="D2" s="84"/>
-      <c r="E2" s="84"/>
-      <c r="F2" s="84"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="84"/>
-      <c r="J2" s="84"/>
+      <c r="B2" s="86"/>
+      <c r="C2" s="86"/>
+      <c r="D2" s="86"/>
+      <c r="E2" s="86"/>
+      <c r="F2" s="86"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="86"/>
+      <c r="J2" s="86"/>
       <c r="K2" s="7"/>
       <c r="L2" s="7"/>
     </row>
@@ -3047,38 +3512,38 @@
       <c r="L3" s="6"/>
     </row>
     <row r="4" spans="1:12" ht="17.25" customHeight="1">
-      <c r="A4" s="89" t="s">
+      <c r="A4" s="91" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="93" t="s">
+      <c r="B4" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="91" t="s">
+      <c r="C4" s="93" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="92"/>
+      <c r="D4" s="94"/>
       <c r="E4" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="91" t="s">
+      <c r="F4" s="93" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="92"/>
-      <c r="H4" s="89" t="s">
+      <c r="G4" s="94"/>
+      <c r="H4" s="91" t="s">
         <v>6</v>
       </c>
-      <c r="I4" s="89" t="s">
+      <c r="I4" s="91" t="s">
         <v>7</v>
       </c>
-      <c r="J4" s="89" t="s">
+      <c r="J4" s="91" t="s">
         <v>8</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
     </row>
     <row r="5" spans="1:12" ht="41.25" customHeight="1">
-      <c r="A5" s="90"/>
-      <c r="B5" s="90"/>
+      <c r="A5" s="92"/>
+      <c r="B5" s="92"/>
       <c r="C5" s="12" t="s">
         <v>9</v>
       </c>
@@ -3094,9 +3559,9 @@
       <c r="G5" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="H5" s="90"/>
-      <c r="I5" s="90"/>
-      <c r="J5" s="90"/>
+      <c r="H5" s="92"/>
+      <c r="I5" s="92"/>
+      <c r="J5" s="92"/>
       <c r="K5" s="11"/>
       <c r="L5" s="11"/>
     </row>
@@ -3353,86 +3818,86 @@
       <c r="L22" s="17"/>
     </row>
     <row r="23" spans="1:12" ht="15" customHeight="1">
-      <c r="A23" s="94"/>
-      <c r="B23" s="84"/>
-      <c r="C23" s="84"/>
-      <c r="D23" s="84"/>
-      <c r="E23" s="84"/>
-      <c r="F23" s="84"/>
-      <c r="G23" s="84"/>
-      <c r="H23" s="84"/>
-      <c r="I23" s="84"/>
-      <c r="J23" s="84"/>
+      <c r="A23" s="96"/>
+      <c r="B23" s="86"/>
+      <c r="C23" s="86"/>
+      <c r="D23" s="86"/>
+      <c r="E23" s="86"/>
+      <c r="F23" s="86"/>
+      <c r="G23" s="86"/>
+      <c r="H23" s="86"/>
+      <c r="I23" s="86"/>
+      <c r="J23" s="86"/>
       <c r="K23" s="19"/>
       <c r="L23" s="19"/>
     </row>
     <row r="24" spans="1:12" ht="15" customHeight="1">
-      <c r="A24" s="87"/>
-      <c r="B24" s="84"/>
-      <c r="C24" s="84"/>
-      <c r="D24" s="84"/>
-      <c r="E24" s="84"/>
-      <c r="F24" s="84"/>
-      <c r="G24" s="84"/>
-      <c r="H24" s="84"/>
-      <c r="I24" s="84"/>
-      <c r="J24" s="84"/>
+      <c r="A24" s="89"/>
+      <c r="B24" s="86"/>
+      <c r="C24" s="86"/>
+      <c r="D24" s="86"/>
+      <c r="E24" s="86"/>
+      <c r="F24" s="86"/>
+      <c r="G24" s="86"/>
+      <c r="H24" s="86"/>
+      <c r="I24" s="86"/>
+      <c r="J24" s="86"/>
       <c r="K24" s="19"/>
       <c r="L24" s="19"/>
     </row>
     <row r="25" spans="1:12" ht="15" customHeight="1">
-      <c r="A25" s="87"/>
-      <c r="B25" s="84"/>
-      <c r="C25" s="84"/>
-      <c r="D25" s="84"/>
-      <c r="E25" s="84"/>
-      <c r="F25" s="84"/>
-      <c r="G25" s="84"/>
-      <c r="H25" s="84"/>
-      <c r="I25" s="84"/>
-      <c r="J25" s="84"/>
+      <c r="A25" s="89"/>
+      <c r="B25" s="86"/>
+      <c r="C25" s="86"/>
+      <c r="D25" s="86"/>
+      <c r="E25" s="86"/>
+      <c r="F25" s="86"/>
+      <c r="G25" s="86"/>
+      <c r="H25" s="86"/>
+      <c r="I25" s="86"/>
+      <c r="J25" s="86"/>
       <c r="K25" s="19"/>
       <c r="L25" s="19"/>
     </row>
     <row r="26" spans="1:12" ht="15" customHeight="1">
-      <c r="A26" s="87"/>
-      <c r="B26" s="84"/>
-      <c r="C26" s="84"/>
-      <c r="D26" s="84"/>
-      <c r="E26" s="84"/>
-      <c r="F26" s="84"/>
-      <c r="G26" s="84"/>
-      <c r="H26" s="84"/>
-      <c r="I26" s="84"/>
-      <c r="J26" s="84"/>
+      <c r="A26" s="89"/>
+      <c r="B26" s="86"/>
+      <c r="C26" s="86"/>
+      <c r="D26" s="86"/>
+      <c r="E26" s="86"/>
+      <c r="F26" s="86"/>
+      <c r="G26" s="86"/>
+      <c r="H26" s="86"/>
+      <c r="I26" s="86"/>
+      <c r="J26" s="86"/>
       <c r="K26" s="19"/>
       <c r="L26" s="19"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A27" s="87"/>
-      <c r="B27" s="84"/>
-      <c r="C27" s="84"/>
-      <c r="D27" s="84"/>
-      <c r="E27" s="84"/>
-      <c r="F27" s="84"/>
-      <c r="G27" s="84"/>
-      <c r="H27" s="84"/>
-      <c r="I27" s="84"/>
-      <c r="J27" s="84"/>
+      <c r="A27" s="89"/>
+      <c r="B27" s="86"/>
+      <c r="C27" s="86"/>
+      <c r="D27" s="86"/>
+      <c r="E27" s="86"/>
+      <c r="F27" s="86"/>
+      <c r="G27" s="86"/>
+      <c r="H27" s="86"/>
+      <c r="I27" s="86"/>
+      <c r="J27" s="86"/>
       <c r="K27" s="6"/>
       <c r="L27" s="6"/>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
-      <c r="A28" s="87"/>
-      <c r="B28" s="84"/>
-      <c r="C28" s="84"/>
-      <c r="D28" s="84"/>
-      <c r="E28" s="84"/>
-      <c r="F28" s="84"/>
-      <c r="G28" s="84"/>
-      <c r="H28" s="84"/>
-      <c r="I28" s="84"/>
-      <c r="J28" s="84"/>
+      <c r="A28" s="89"/>
+      <c r="B28" s="86"/>
+      <c r="C28" s="86"/>
+      <c r="D28" s="86"/>
+      <c r="E28" s="86"/>
+      <c r="F28" s="86"/>
+      <c r="G28" s="86"/>
+      <c r="H28" s="86"/>
+      <c r="I28" s="86"/>
+      <c r="J28" s="86"/>
       <c r="K28" s="6"/>
       <c r="L28" s="6"/>
     </row>
@@ -4473,7 +4938,7 @@
   <dimension ref="A1:W100"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="80" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
-      <selection activeCell="AA16" sqref="AA16"/>
+      <selection activeCell="Z11" sqref="Z11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.375" defaultRowHeight="15" customHeight="1"/>
@@ -4500,25 +4965,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" ht="31.5" customHeight="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="133" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
-      <c r="N1" s="109" t="s">
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
+      <c r="N1" s="125" t="s">
         <v>96</v>
       </c>
-      <c r="O1" s="109"/>
+      <c r="O1" s="125"/>
       <c r="P1" s="5" t="s">
         <v>16</v>
       </c>
@@ -4550,14 +5015,14 @@
       <c r="C2" s="81"/>
       <c r="D2" s="81"/>
       <c r="E2" s="23"/>
-      <c r="F2" s="119"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="84"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="86"/>
       <c r="N2" s="5" t="s">
         <v>22</v>
       </c>
@@ -4588,27 +5053,27 @@
       <c r="W2" s="24"/>
     </row>
     <row r="3" spans="1:23" ht="22.5" customHeight="1">
-      <c r="A3" s="116" t="s">
+      <c r="A3" s="131" t="s">
         <v>24</v>
       </c>
-      <c r="B3" s="117" t="s">
+      <c r="B3" s="132" t="s">
         <v>89</v>
       </c>
-      <c r="C3" s="112"/>
-      <c r="D3" s="113"/>
-      <c r="E3" s="111" t="s">
+      <c r="C3" s="128"/>
+      <c r="D3" s="129"/>
+      <c r="E3" s="127" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="112"/>
-      <c r="G3" s="113"/>
-      <c r="H3" s="122" t="s">
+      <c r="F3" s="128"/>
+      <c r="G3" s="129"/>
+      <c r="H3" s="137" t="s">
         <v>105</v>
       </c>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="124"/>
+      <c r="I3" s="138"/>
+      <c r="J3" s="138"/>
+      <c r="K3" s="138"/>
+      <c r="L3" s="138"/>
+      <c r="M3" s="139"/>
       <c r="N3" s="22">
         <v>2700</v>
       </c>
@@ -4641,19 +5106,19 @@
       <c r="W3" s="24"/>
     </row>
     <row r="4" spans="1:23" ht="22.5" customHeight="1">
-      <c r="A4" s="115"/>
-      <c r="B4" s="101"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="102"/>
-      <c r="E4" s="101"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="102"/>
-      <c r="H4" s="125"/>
-      <c r="I4" s="126"/>
-      <c r="J4" s="126"/>
-      <c r="K4" s="126"/>
-      <c r="L4" s="126"/>
-      <c r="M4" s="127"/>
+      <c r="A4" s="130"/>
+      <c r="B4" s="110"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="112"/>
+      <c r="E4" s="110"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="112"/>
+      <c r="H4" s="140"/>
+      <c r="I4" s="141"/>
+      <c r="J4" s="141"/>
+      <c r="K4" s="141"/>
+      <c r="L4" s="141"/>
+      <c r="M4" s="142"/>
       <c r="N4" s="22">
         <v>2900</v>
       </c>
@@ -4676,19 +5141,19 @@
       <c r="W4" s="5"/>
     </row>
     <row r="5" spans="1:23" ht="22.5" customHeight="1">
-      <c r="A5" s="115"/>
-      <c r="B5" s="101"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="102"/>
-      <c r="E5" s="101"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="102"/>
-      <c r="H5" s="125"/>
-      <c r="I5" s="126"/>
-      <c r="J5" s="126"/>
-      <c r="K5" s="126"/>
-      <c r="L5" s="126"/>
-      <c r="M5" s="127"/>
+      <c r="A5" s="130"/>
+      <c r="B5" s="110"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="112"/>
+      <c r="E5" s="110"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="112"/>
+      <c r="H5" s="140"/>
+      <c r="I5" s="141"/>
+      <c r="J5" s="141"/>
+      <c r="K5" s="141"/>
+      <c r="L5" s="141"/>
+      <c r="M5" s="142"/>
       <c r="N5" s="22">
         <v>550</v>
       </c>
@@ -4709,23 +5174,23 @@
       <c r="W5" s="5"/>
     </row>
     <row r="6" spans="1:23" ht="22.5" customHeight="1">
-      <c r="A6" s="95" t="s">
+      <c r="A6" s="118" t="s">
         <v>27</v>
       </c>
-      <c r="B6" s="110" t="s">
+      <c r="B6" s="126" t="s">
         <v>90</v>
       </c>
-      <c r="C6" s="99"/>
-      <c r="D6" s="100"/>
-      <c r="E6" s="101"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="102"/>
-      <c r="H6" s="125"/>
-      <c r="I6" s="126"/>
-      <c r="J6" s="126"/>
-      <c r="K6" s="126"/>
-      <c r="L6" s="126"/>
-      <c r="M6" s="127"/>
+      <c r="C6" s="100"/>
+      <c r="D6" s="114"/>
+      <c r="E6" s="110"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="112"/>
+      <c r="H6" s="140"/>
+      <c r="I6" s="141"/>
+      <c r="J6" s="141"/>
+      <c r="K6" s="141"/>
+      <c r="L6" s="141"/>
+      <c r="M6" s="142"/>
       <c r="N6" s="22">
         <v>390</v>
       </c>
@@ -4746,19 +5211,19 @@
       <c r="W6" s="5"/>
     </row>
     <row r="7" spans="1:23" ht="22.5" customHeight="1">
-      <c r="A7" s="96"/>
-      <c r="B7" s="101"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="102"/>
-      <c r="E7" s="101"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="102"/>
-      <c r="H7" s="125"/>
-      <c r="I7" s="126"/>
-      <c r="J7" s="126"/>
-      <c r="K7" s="126"/>
-      <c r="L7" s="126"/>
-      <c r="M7" s="127"/>
+      <c r="A7" s="119"/>
+      <c r="B7" s="110"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="112"/>
+      <c r="E7" s="110"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="112"/>
+      <c r="H7" s="140"/>
+      <c r="I7" s="141"/>
+      <c r="J7" s="141"/>
+      <c r="K7" s="141"/>
+      <c r="L7" s="141"/>
+      <c r="M7" s="142"/>
       <c r="N7" s="22">
         <v>31</v>
       </c>
@@ -4777,19 +5242,19 @@
       <c r="W7" s="5"/>
     </row>
     <row r="8" spans="1:23" ht="22.5" customHeight="1">
-      <c r="A8" s="96"/>
-      <c r="B8" s="101"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="102"/>
-      <c r="E8" s="101"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="102"/>
-      <c r="H8" s="125"/>
-      <c r="I8" s="126"/>
-      <c r="J8" s="126"/>
-      <c r="K8" s="126"/>
-      <c r="L8" s="126"/>
-      <c r="M8" s="127"/>
+      <c r="A8" s="119"/>
+      <c r="B8" s="110"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="112"/>
+      <c r="E8" s="110"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="112"/>
+      <c r="H8" s="140"/>
+      <c r="I8" s="141"/>
+      <c r="J8" s="141"/>
+      <c r="K8" s="141"/>
+      <c r="L8" s="141"/>
+      <c r="M8" s="142"/>
       <c r="N8" s="30"/>
       <c r="O8" s="5" t="s">
         <v>28</v>
@@ -4812,24 +5277,24 @@
       <c r="W8" s="5"/>
     </row>
     <row r="9" spans="1:23" ht="22.5" customHeight="1">
-      <c r="A9" s="95" t="s">
+      <c r="A9" s="118" t="s">
         <v>31</v>
       </c>
-      <c r="B9" s="98">
+      <c r="B9" s="121">
         <f>L12</f>
         <v>0</v>
       </c>
-      <c r="C9" s="99"/>
-      <c r="D9" s="100"/>
-      <c r="E9" s="101"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="102"/>
-      <c r="H9" s="125"/>
-      <c r="I9" s="126"/>
-      <c r="J9" s="126"/>
-      <c r="K9" s="126"/>
-      <c r="L9" s="126"/>
-      <c r="M9" s="127"/>
+      <c r="C9" s="100"/>
+      <c r="D9" s="114"/>
+      <c r="E9" s="110"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="112"/>
+      <c r="H9" s="140"/>
+      <c r="I9" s="141"/>
+      <c r="J9" s="141"/>
+      <c r="K9" s="141"/>
+      <c r="L9" s="141"/>
+      <c r="M9" s="142"/>
       <c r="N9" s="22">
         <f>SUM(M3:M8)*Q9</f>
         <v>0</v>
@@ -4856,19 +5321,19 @@
       <c r="W9" s="5"/>
     </row>
     <row r="10" spans="1:23" ht="15.75" customHeight="1">
-      <c r="A10" s="96"/>
-      <c r="B10" s="101"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="102"/>
-      <c r="E10" s="101"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="102"/>
-      <c r="H10" s="125"/>
-      <c r="I10" s="126"/>
-      <c r="J10" s="126"/>
-      <c r="K10" s="126"/>
-      <c r="L10" s="126"/>
-      <c r="M10" s="127"/>
+      <c r="A10" s="119"/>
+      <c r="B10" s="110"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="112"/>
+      <c r="E10" s="110"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="112"/>
+      <c r="H10" s="140"/>
+      <c r="I10" s="141"/>
+      <c r="J10" s="141"/>
+      <c r="K10" s="141"/>
+      <c r="L10" s="141"/>
+      <c r="M10" s="142"/>
       <c r="N10" s="22"/>
       <c r="O10" s="31"/>
       <c r="P10" s="24"/>
@@ -4885,19 +5350,19 @@
       <c r="W10" s="5"/>
     </row>
     <row r="11" spans="1:23" ht="18" customHeight="1">
-      <c r="A11" s="96"/>
-      <c r="B11" s="101"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="102"/>
-      <c r="E11" s="101"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="102"/>
-      <c r="H11" s="125"/>
-      <c r="I11" s="126"/>
-      <c r="J11" s="126"/>
-      <c r="K11" s="126"/>
-      <c r="L11" s="126"/>
-      <c r="M11" s="127"/>
+      <c r="A11" s="119"/>
+      <c r="B11" s="110"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="112"/>
+      <c r="E11" s="110"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="112"/>
+      <c r="H11" s="140"/>
+      <c r="I11" s="141"/>
+      <c r="J11" s="141"/>
+      <c r="K11" s="141"/>
+      <c r="L11" s="141"/>
+      <c r="M11" s="142"/>
       <c r="N11" s="22"/>
       <c r="O11" s="31"/>
       <c r="P11" s="24"/>
@@ -4914,19 +5379,19 @@
       <c r="W11" s="5"/>
     </row>
     <row r="12" spans="1:23" ht="19.5" customHeight="1">
-      <c r="A12" s="96"/>
-      <c r="B12" s="101"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="102"/>
-      <c r="E12" s="101"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="102"/>
-      <c r="H12" s="125"/>
-      <c r="I12" s="126"/>
-      <c r="J12" s="126"/>
-      <c r="K12" s="126"/>
-      <c r="L12" s="126"/>
-      <c r="M12" s="127"/>
+      <c r="A12" s="119"/>
+      <c r="B12" s="110"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="112"/>
+      <c r="E12" s="110"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="112"/>
+      <c r="H12" s="140"/>
+      <c r="I12" s="141"/>
+      <c r="J12" s="141"/>
+      <c r="K12" s="141"/>
+      <c r="L12" s="141"/>
+      <c r="M12" s="142"/>
       <c r="N12" s="5" t="s">
         <v>32</v>
       </c>
@@ -4943,19 +5408,19 @@
       <c r="W12" s="5"/>
     </row>
     <row r="13" spans="1:23" ht="18.75" customHeight="1" thickBot="1">
-      <c r="A13" s="97"/>
-      <c r="B13" s="103"/>
-      <c r="C13" s="104"/>
-      <c r="D13" s="105"/>
-      <c r="E13" s="103"/>
-      <c r="F13" s="104"/>
-      <c r="G13" s="105"/>
-      <c r="H13" s="128"/>
-      <c r="I13" s="129"/>
-      <c r="J13" s="129"/>
-      <c r="K13" s="129"/>
-      <c r="L13" s="129"/>
-      <c r="M13" s="130"/>
+      <c r="A13" s="120"/>
+      <c r="B13" s="102"/>
+      <c r="C13" s="103"/>
+      <c r="D13" s="115"/>
+      <c r="E13" s="102"/>
+      <c r="F13" s="103"/>
+      <c r="G13" s="115"/>
+      <c r="H13" s="143"/>
+      <c r="I13" s="144"/>
+      <c r="J13" s="144"/>
+      <c r="K13" s="144"/>
+      <c r="L13" s="144"/>
+      <c r="M13" s="145"/>
       <c r="N13" s="32"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5" t="s">
@@ -4980,29 +5445,29 @@
       <c r="W13" s="5"/>
     </row>
     <row r="14" spans="1:23" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A14" s="114" t="s">
+      <c r="A14" s="106" t="s">
         <v>39</v>
       </c>
-      <c r="B14" s="141" t="str">
+      <c r="B14" s="113" t="str">
         <f>"受益面積"&amp;O6&amp;"公頃"</f>
         <v>受益面積20公頃</v>
       </c>
-      <c r="C14" s="99"/>
-      <c r="D14" s="100"/>
-      <c r="E14" s="138" t="s">
+      <c r="C14" s="100"/>
+      <c r="D14" s="114"/>
+      <c r="E14" s="108" t="s">
         <v>40</v>
       </c>
-      <c r="F14" s="84"/>
-      <c r="G14" s="102"/>
-      <c r="H14" s="138" t="s">
+      <c r="F14" s="86"/>
+      <c r="G14" s="112"/>
+      <c r="H14" s="108" t="s">
         <v>106</v>
       </c>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="84"/>
-      <c r="M14" s="139"/>
-      <c r="N14" s="106" t="s">
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="109"/>
+      <c r="N14" s="122" t="s">
         <v>41</v>
       </c>
       <c r="O14" s="34" t="s">
@@ -5036,20 +5501,20 @@
       <c r="W14" s="5"/>
     </row>
     <row r="15" spans="1:23" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A15" s="137"/>
-      <c r="B15" s="103"/>
-      <c r="C15" s="104"/>
-      <c r="D15" s="105"/>
-      <c r="E15" s="101"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="102"/>
-      <c r="H15" s="101"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="139"/>
-      <c r="N15" s="108"/>
+      <c r="A15" s="107"/>
+      <c r="B15" s="102"/>
+      <c r="C15" s="103"/>
+      <c r="D15" s="115"/>
+      <c r="E15" s="110"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="112"/>
+      <c r="H15" s="110"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="109"/>
+      <c r="N15" s="124"/>
       <c r="O15" s="34" t="s">
         <v>43</v>
       </c>
@@ -5082,26 +5547,26 @@
       <c r="W15" s="5"/>
     </row>
     <row r="16" spans="1:23" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A16" s="114" t="s">
+      <c r="A16" s="106" t="s">
         <v>44</v>
       </c>
-      <c r="B16" s="136" t="s">
+      <c r="B16" s="105" t="s">
         <v>45</v>
       </c>
       <c r="C16" s="44" t="s">
         <v>46</v>
       </c>
       <c r="D16" s="45"/>
-      <c r="E16" s="101"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="102"/>
-      <c r="H16" s="101"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="84"/>
-      <c r="M16" s="139"/>
-      <c r="N16" s="106" t="s">
+      <c r="E16" s="110"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="112"/>
+      <c r="H16" s="110"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="109"/>
+      <c r="N16" s="122" t="s">
         <v>47</v>
       </c>
       <c r="O16" s="46" t="s">
@@ -5136,22 +5601,22 @@
       <c r="W16" s="5"/>
     </row>
     <row r="17" spans="1:23" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A17" s="115"/>
-      <c r="B17" s="90"/>
+      <c r="A17" s="130"/>
+      <c r="B17" s="92"/>
       <c r="C17" s="44" t="s">
         <v>48</v>
       </c>
       <c r="D17" s="45"/>
-      <c r="E17" s="101"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="102"/>
-      <c r="H17" s="101"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="84"/>
-      <c r="K17" s="84"/>
-      <c r="L17" s="84"/>
-      <c r="M17" s="139"/>
-      <c r="N17" s="107"/>
+      <c r="E17" s="110"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="112"/>
+      <c r="H17" s="110"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="109"/>
+      <c r="N17" s="123"/>
       <c r="O17" s="46" t="s">
         <v>49</v>
       </c>
@@ -5184,24 +5649,24 @@
       <c r="W17" s="5"/>
     </row>
     <row r="18" spans="1:23" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A18" s="115"/>
-      <c r="B18" s="136" t="s">
+      <c r="A18" s="130"/>
+      <c r="B18" s="105" t="s">
         <v>50</v>
       </c>
       <c r="C18" s="44" t="s">
         <v>46</v>
       </c>
       <c r="D18" s="45"/>
-      <c r="E18" s="101"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="102"/>
-      <c r="H18" s="101"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="84"/>
-      <c r="L18" s="84"/>
-      <c r="M18" s="139"/>
-      <c r="N18" s="107"/>
+      <c r="E18" s="110"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="112"/>
+      <c r="H18" s="110"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="109"/>
+      <c r="N18" s="123"/>
       <c r="O18" s="46" t="s">
         <v>19</v>
       </c>
@@ -5234,22 +5699,22 @@
       <c r="W18" s="5"/>
     </row>
     <row r="19" spans="1:23" ht="33.75" customHeight="1" thickBot="1">
-      <c r="A19" s="115"/>
-      <c r="B19" s="140"/>
+      <c r="A19" s="130"/>
+      <c r="B19" s="111"/>
       <c r="C19" s="43" t="s">
         <v>48</v>
       </c>
       <c r="D19" s="50"/>
-      <c r="E19" s="101"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="102"/>
-      <c r="H19" s="101"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="84"/>
-      <c r="M19" s="139"/>
-      <c r="N19" s="108"/>
+      <c r="E19" s="110"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="112"/>
+      <c r="H19" s="110"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="86"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="109"/>
+      <c r="N19" s="124"/>
       <c r="O19" s="46" t="s">
         <v>42</v>
       </c>
@@ -5281,27 +5746,27 @@
       <c r="W19" s="5"/>
     </row>
     <row r="20" spans="1:23" ht="22.5" customHeight="1">
-      <c r="A20" s="114" t="s">
+      <c r="A20" s="106" t="s">
         <v>51</v>
       </c>
       <c r="B20" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="C20" s="142" t="s">
+      <c r="C20" s="116" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="143"/>
-      <c r="E20" s="133" t="s">
+      <c r="D20" s="117"/>
+      <c r="E20" s="99" t="s">
         <v>54</v>
       </c>
-      <c r="F20" s="99"/>
-      <c r="G20" s="99"/>
-      <c r="H20" s="99"/>
-      <c r="I20" s="99"/>
-      <c r="J20" s="99"/>
-      <c r="K20" s="99"/>
-      <c r="L20" s="99"/>
-      <c r="M20" s="134"/>
+      <c r="F20" s="100"/>
+      <c r="G20" s="100"/>
+      <c r="H20" s="100"/>
+      <c r="I20" s="100"/>
+      <c r="J20" s="100"/>
+      <c r="K20" s="100"/>
+      <c r="L20" s="100"/>
+      <c r="M20" s="101"/>
       <c r="N20" s="5"/>
       <c r="O20" s="5"/>
       <c r="P20" s="5"/>
@@ -5317,23 +5782,23 @@
       <c r="W20" s="5"/>
     </row>
     <row r="21" spans="1:23" ht="22.5" customHeight="1">
-      <c r="A21" s="137"/>
+      <c r="A21" s="107"/>
       <c r="B21" s="80" t="s">
         <v>52</v>
       </c>
-      <c r="C21" s="142" t="s">
+      <c r="C21" s="116" t="s">
         <v>55</v>
       </c>
-      <c r="D21" s="143"/>
-      <c r="E21" s="103"/>
-      <c r="F21" s="104"/>
-      <c r="G21" s="104"/>
-      <c r="H21" s="104"/>
-      <c r="I21" s="104"/>
-      <c r="J21" s="104"/>
-      <c r="K21" s="104"/>
-      <c r="L21" s="104"/>
-      <c r="M21" s="135"/>
+      <c r="D21" s="117"/>
+      <c r="E21" s="102"/>
+      <c r="F21" s="103"/>
+      <c r="G21" s="103"/>
+      <c r="H21" s="103"/>
+      <c r="I21" s="103"/>
+      <c r="J21" s="103"/>
+      <c r="K21" s="103"/>
+      <c r="L21" s="103"/>
+      <c r="M21" s="104"/>
       <c r="N21" s="5"/>
       <c r="O21" s="21"/>
       <c r="P21" s="21"/>
@@ -5346,23 +5811,23 @@
       <c r="W21" s="5"/>
     </row>
     <row r="22" spans="1:23" ht="30.75" customHeight="1" thickBot="1">
-      <c r="A22" s="131" t="s">
+      <c r="A22" s="97" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="132"/>
-      <c r="C22" s="132"/>
-      <c r="D22" s="132"/>
-      <c r="E22" s="132"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="98"/>
       <c r="F22" s="51"/>
       <c r="G22" s="51" t="s">
         <v>57</v>
       </c>
-      <c r="H22" s="150"/>
-      <c r="I22" s="150"/>
-      <c r="J22" s="150"/>
-      <c r="K22" s="150"/>
-      <c r="L22" s="150"/>
-      <c r="M22" s="151"/>
+      <c r="H22" s="83"/>
+      <c r="I22" s="83"/>
+      <c r="J22" s="83"/>
+      <c r="K22" s="83"/>
+      <c r="L22" s="83"/>
+      <c r="M22" s="84"/>
       <c r="N22" s="5"/>
       <c r="O22" s="5"/>
       <c r="P22" s="5"/>
@@ -7328,17 +7793,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="A22:E22"/>
-    <mergeCell ref="E20:M21"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="H14:M19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="E14:G19"/>
-    <mergeCell ref="B14:D15"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C21:D21"/>
     <mergeCell ref="A9:A13"/>
     <mergeCell ref="B9:D13"/>
     <mergeCell ref="N16:N19"/>
@@ -7355,6 +7809,17 @@
     <mergeCell ref="I2:K2"/>
     <mergeCell ref="L2:M2"/>
     <mergeCell ref="H3:M13"/>
+    <mergeCell ref="A22:E22"/>
+    <mergeCell ref="E20:M21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="A14:A15"/>
+    <mergeCell ref="H14:M19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="E14:G19"/>
+    <mergeCell ref="B14:D15"/>
+    <mergeCell ref="A20:A21"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C21:D21"/>
   </mergeCells>
   <phoneticPr fontId="24" type="noConversion"/>
   <dataValidations count="1">
@@ -7401,21 +7866,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="31.5" customHeight="1">
-      <c r="A1" s="118" t="s">
+      <c r="A1" s="133" t="s">
         <v>58</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="84"/>
-      <c r="E1" s="84"/>
-      <c r="F1" s="84"/>
-      <c r="G1" s="84"/>
-      <c r="H1" s="84"/>
-      <c r="I1" s="84"/>
-      <c r="J1" s="84"/>
-      <c r="K1" s="84"/>
-      <c r="L1" s="84"/>
-      <c r="M1" s="84"/>
+      <c r="B1" s="86"/>
+      <c r="C1" s="86"/>
+      <c r="D1" s="86"/>
+      <c r="E1" s="86"/>
+      <c r="F1" s="86"/>
+      <c r="G1" s="86"/>
+      <c r="H1" s="86"/>
+      <c r="I1" s="86"/>
+      <c r="J1" s="86"/>
+      <c r="K1" s="86"/>
+      <c r="L1" s="86"/>
+      <c r="M1" s="86"/>
       <c r="N1" s="5"/>
       <c r="O1" s="5"/>
       <c r="P1" s="5"/>
@@ -7427,23 +7892,23 @@
       <c r="V1" s="5"/>
     </row>
     <row r="2" spans="1:22" ht="24.75" customHeight="1">
-      <c r="A2" s="149" t="s">
+      <c r="A2" s="151" t="s">
         <v>21</v>
       </c>
-      <c r="B2" s="132"/>
-      <c r="C2" s="132"/>
-      <c r="D2" s="132"/>
+      <c r="B2" s="98"/>
+      <c r="C2" s="98"/>
+      <c r="D2" s="98"/>
       <c r="E2" s="73" t="s">
         <v>59</v>
       </c>
-      <c r="F2" s="119"/>
-      <c r="G2" s="84"/>
-      <c r="H2" s="84"/>
-      <c r="I2" s="120"/>
-      <c r="J2" s="84"/>
-      <c r="K2" s="84"/>
-      <c r="L2" s="121"/>
-      <c r="M2" s="84"/>
+      <c r="F2" s="134"/>
+      <c r="G2" s="86"/>
+      <c r="H2" s="86"/>
+      <c r="I2" s="135"/>
+      <c r="J2" s="86"/>
+      <c r="K2" s="86"/>
+      <c r="L2" s="136"/>
+      <c r="M2" s="86"/>
       <c r="N2" s="5"/>
       <c r="O2" s="5"/>
       <c r="P2" s="5"/>
@@ -7455,19 +7920,19 @@
       <c r="V2" s="5"/>
     </row>
     <row r="3" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A3" s="144"/>
-      <c r="B3" s="112"/>
-      <c r="C3" s="112"/>
-      <c r="D3" s="112"/>
-      <c r="E3" s="112"/>
-      <c r="F3" s="112"/>
-      <c r="G3" s="112"/>
-      <c r="H3" s="112"/>
-      <c r="I3" s="112"/>
-      <c r="J3" s="112"/>
-      <c r="K3" s="112"/>
-      <c r="L3" s="112"/>
-      <c r="M3" s="145"/>
+      <c r="A3" s="146"/>
+      <c r="B3" s="128"/>
+      <c r="C3" s="128"/>
+      <c r="D3" s="128"/>
+      <c r="E3" s="128"/>
+      <c r="F3" s="128"/>
+      <c r="G3" s="128"/>
+      <c r="H3" s="128"/>
+      <c r="I3" s="128"/>
+      <c r="J3" s="128"/>
+      <c r="K3" s="128"/>
+      <c r="L3" s="128"/>
+      <c r="M3" s="147"/>
       <c r="N3" s="5"/>
       <c r="O3" s="5"/>
       <c r="P3" s="5"/>
@@ -7479,19 +7944,19 @@
       <c r="V3" s="5"/>
     </row>
     <row r="4" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A4" s="146"/>
-      <c r="B4" s="84"/>
-      <c r="C4" s="84"/>
-      <c r="D4" s="84"/>
-      <c r="E4" s="84"/>
-      <c r="F4" s="84"/>
-      <c r="G4" s="84"/>
-      <c r="H4" s="84"/>
-      <c r="I4" s="84"/>
-      <c r="J4" s="84"/>
-      <c r="K4" s="84"/>
-      <c r="L4" s="84"/>
-      <c r="M4" s="139"/>
+      <c r="A4" s="148"/>
+      <c r="B4" s="86"/>
+      <c r="C4" s="86"/>
+      <c r="D4" s="86"/>
+      <c r="E4" s="86"/>
+      <c r="F4" s="86"/>
+      <c r="G4" s="86"/>
+      <c r="H4" s="86"/>
+      <c r="I4" s="86"/>
+      <c r="J4" s="86"/>
+      <c r="K4" s="86"/>
+      <c r="L4" s="86"/>
+      <c r="M4" s="109"/>
       <c r="N4" s="5"/>
       <c r="O4" s="5"/>
       <c r="P4" s="5"/>
@@ -7503,19 +7968,19 @@
       <c r="V4" s="21"/>
     </row>
     <row r="5" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A5" s="146"/>
-      <c r="B5" s="84"/>
-      <c r="C5" s="84"/>
-      <c r="D5" s="84"/>
-      <c r="E5" s="84"/>
-      <c r="F5" s="84"/>
-      <c r="G5" s="84"/>
-      <c r="H5" s="84"/>
-      <c r="I5" s="84"/>
-      <c r="J5" s="84"/>
-      <c r="K5" s="84"/>
-      <c r="L5" s="84"/>
-      <c r="M5" s="139"/>
+      <c r="A5" s="148"/>
+      <c r="B5" s="86"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="86"/>
+      <c r="E5" s="86"/>
+      <c r="F5" s="86"/>
+      <c r="G5" s="86"/>
+      <c r="H5" s="86"/>
+      <c r="I5" s="86"/>
+      <c r="J5" s="86"/>
+      <c r="K5" s="86"/>
+      <c r="L5" s="86"/>
+      <c r="M5" s="109"/>
       <c r="N5" s="5"/>
       <c r="O5" s="5"/>
       <c r="P5" s="5"/>
@@ -7527,19 +7992,19 @@
       <c r="V5" s="5"/>
     </row>
     <row r="6" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A6" s="146"/>
-      <c r="B6" s="84"/>
-      <c r="C6" s="84"/>
-      <c r="D6" s="84"/>
-      <c r="E6" s="84"/>
-      <c r="F6" s="84"/>
-      <c r="G6" s="84"/>
-      <c r="H6" s="84"/>
-      <c r="I6" s="84"/>
-      <c r="J6" s="84"/>
-      <c r="K6" s="84"/>
-      <c r="L6" s="84"/>
-      <c r="M6" s="139"/>
+      <c r="A6" s="148"/>
+      <c r="B6" s="86"/>
+      <c r="C6" s="86"/>
+      <c r="D6" s="86"/>
+      <c r="E6" s="86"/>
+      <c r="F6" s="86"/>
+      <c r="G6" s="86"/>
+      <c r="H6" s="86"/>
+      <c r="I6" s="86"/>
+      <c r="J6" s="86"/>
+      <c r="K6" s="86"/>
+      <c r="L6" s="86"/>
+      <c r="M6" s="109"/>
       <c r="N6" s="5"/>
       <c r="O6" s="5"/>
       <c r="P6" s="5"/>
@@ -7551,19 +8016,19 @@
       <c r="V6" s="5"/>
     </row>
     <row r="7" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A7" s="146"/>
-      <c r="B7" s="84"/>
-      <c r="C7" s="84"/>
-      <c r="D7" s="84"/>
-      <c r="E7" s="84"/>
-      <c r="F7" s="84"/>
-      <c r="G7" s="84"/>
-      <c r="H7" s="84"/>
-      <c r="I7" s="84"/>
-      <c r="J7" s="84"/>
-      <c r="K7" s="84"/>
-      <c r="L7" s="84"/>
-      <c r="M7" s="139"/>
+      <c r="A7" s="148"/>
+      <c r="B7" s="86"/>
+      <c r="C7" s="86"/>
+      <c r="D7" s="86"/>
+      <c r="E7" s="86"/>
+      <c r="F7" s="86"/>
+      <c r="G7" s="86"/>
+      <c r="H7" s="86"/>
+      <c r="I7" s="86"/>
+      <c r="J7" s="86"/>
+      <c r="K7" s="86"/>
+      <c r="L7" s="86"/>
+      <c r="M7" s="109"/>
       <c r="N7" s="5"/>
       <c r="O7" s="5"/>
       <c r="P7" s="5"/>
@@ -7575,19 +8040,19 @@
       <c r="V7" s="5"/>
     </row>
     <row r="8" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A8" s="146"/>
-      <c r="B8" s="84"/>
-      <c r="C8" s="84"/>
-      <c r="D8" s="84"/>
-      <c r="E8" s="84"/>
-      <c r="F8" s="84"/>
-      <c r="G8" s="84"/>
-      <c r="H8" s="84"/>
-      <c r="I8" s="84"/>
-      <c r="J8" s="84"/>
-      <c r="K8" s="84"/>
-      <c r="L8" s="84"/>
-      <c r="M8" s="139"/>
+      <c r="A8" s="148"/>
+      <c r="B8" s="86"/>
+      <c r="C8" s="86"/>
+      <c r="D8" s="86"/>
+      <c r="E8" s="86"/>
+      <c r="F8" s="86"/>
+      <c r="G8" s="86"/>
+      <c r="H8" s="86"/>
+      <c r="I8" s="86"/>
+      <c r="J8" s="86"/>
+      <c r="K8" s="86"/>
+      <c r="L8" s="86"/>
+      <c r="M8" s="109"/>
       <c r="N8" s="5"/>
       <c r="O8" s="5"/>
       <c r="P8" s="5"/>
@@ -7599,19 +8064,19 @@
       <c r="V8" s="5"/>
     </row>
     <row r="9" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A9" s="146"/>
-      <c r="B9" s="84"/>
-      <c r="C9" s="84"/>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="84"/>
-      <c r="K9" s="84"/>
-      <c r="L9" s="84"/>
-      <c r="M9" s="139"/>
+      <c r="A9" s="148"/>
+      <c r="B9" s="86"/>
+      <c r="C9" s="86"/>
+      <c r="D9" s="86"/>
+      <c r="E9" s="86"/>
+      <c r="F9" s="86"/>
+      <c r="G9" s="86"/>
+      <c r="H9" s="86"/>
+      <c r="I9" s="86"/>
+      <c r="J9" s="86"/>
+      <c r="K9" s="86"/>
+      <c r="L9" s="86"/>
+      <c r="M9" s="109"/>
       <c r="N9" s="5"/>
       <c r="O9" s="5"/>
       <c r="P9" s="5"/>
@@ -7623,19 +8088,19 @@
       <c r="V9" s="5"/>
     </row>
     <row r="10" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A10" s="146"/>
-      <c r="B10" s="84"/>
-      <c r="C10" s="84"/>
-      <c r="D10" s="84"/>
-      <c r="E10" s="84"/>
-      <c r="F10" s="84"/>
-      <c r="G10" s="84"/>
-      <c r="H10" s="84"/>
-      <c r="I10" s="84"/>
-      <c r="J10" s="84"/>
-      <c r="K10" s="84"/>
-      <c r="L10" s="84"/>
-      <c r="M10" s="139"/>
+      <c r="A10" s="148"/>
+      <c r="B10" s="86"/>
+      <c r="C10" s="86"/>
+      <c r="D10" s="86"/>
+      <c r="E10" s="86"/>
+      <c r="F10" s="86"/>
+      <c r="G10" s="86"/>
+      <c r="H10" s="86"/>
+      <c r="I10" s="86"/>
+      <c r="J10" s="86"/>
+      <c r="K10" s="86"/>
+      <c r="L10" s="86"/>
+      <c r="M10" s="109"/>
       <c r="N10" s="5"/>
       <c r="O10" s="5"/>
       <c r="P10" s="5"/>
@@ -7647,19 +8112,19 @@
       <c r="V10" s="5"/>
     </row>
     <row r="11" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A11" s="146"/>
-      <c r="B11" s="84"/>
-      <c r="C11" s="84"/>
-      <c r="D11" s="84"/>
-      <c r="E11" s="84"/>
-      <c r="F11" s="84"/>
-      <c r="G11" s="84"/>
-      <c r="H11" s="84"/>
-      <c r="I11" s="84"/>
-      <c r="J11" s="84"/>
-      <c r="K11" s="84"/>
-      <c r="L11" s="84"/>
-      <c r="M11" s="139"/>
+      <c r="A11" s="148"/>
+      <c r="B11" s="86"/>
+      <c r="C11" s="86"/>
+      <c r="D11" s="86"/>
+      <c r="E11" s="86"/>
+      <c r="F11" s="86"/>
+      <c r="G11" s="86"/>
+      <c r="H11" s="86"/>
+      <c r="I11" s="86"/>
+      <c r="J11" s="86"/>
+      <c r="K11" s="86"/>
+      <c r="L11" s="86"/>
+      <c r="M11" s="109"/>
       <c r="N11" s="5"/>
       <c r="O11" s="5"/>
       <c r="P11" s="5"/>
@@ -7671,19 +8136,19 @@
       <c r="V11" s="5"/>
     </row>
     <row r="12" spans="1:22" ht="33.75" customHeight="1">
-      <c r="A12" s="146"/>
-      <c r="B12" s="84"/>
-      <c r="C12" s="84"/>
-      <c r="D12" s="84"/>
-      <c r="E12" s="84"/>
-      <c r="F12" s="84"/>
-      <c r="G12" s="84"/>
-      <c r="H12" s="84"/>
-      <c r="I12" s="84"/>
-      <c r="J12" s="84"/>
-      <c r="K12" s="84"/>
-      <c r="L12" s="84"/>
-      <c r="M12" s="139"/>
+      <c r="A12" s="148"/>
+      <c r="B12" s="86"/>
+      <c r="C12" s="86"/>
+      <c r="D12" s="86"/>
+      <c r="E12" s="86"/>
+      <c r="F12" s="86"/>
+      <c r="G12" s="86"/>
+      <c r="H12" s="86"/>
+      <c r="I12" s="86"/>
+      <c r="J12" s="86"/>
+      <c r="K12" s="86"/>
+      <c r="L12" s="86"/>
+      <c r="M12" s="109"/>
       <c r="N12" s="5"/>
       <c r="O12" s="5"/>
       <c r="P12" s="5"/>
@@ -7695,19 +8160,19 @@
       <c r="V12" s="5"/>
     </row>
     <row r="13" spans="1:22" ht="33.75" customHeight="1">
-      <c r="A13" s="146"/>
-      <c r="B13" s="84"/>
-      <c r="C13" s="84"/>
-      <c r="D13" s="84"/>
-      <c r="E13" s="84"/>
-      <c r="F13" s="84"/>
-      <c r="G13" s="84"/>
-      <c r="H13" s="84"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="84"/>
-      <c r="K13" s="84"/>
-      <c r="L13" s="84"/>
-      <c r="M13" s="139"/>
+      <c r="A13" s="148"/>
+      <c r="B13" s="86"/>
+      <c r="C13" s="86"/>
+      <c r="D13" s="86"/>
+      <c r="E13" s="86"/>
+      <c r="F13" s="86"/>
+      <c r="G13" s="86"/>
+      <c r="H13" s="86"/>
+      <c r="I13" s="86"/>
+      <c r="J13" s="86"/>
+      <c r="K13" s="86"/>
+      <c r="L13" s="86"/>
+      <c r="M13" s="109"/>
       <c r="N13" s="5"/>
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
@@ -7719,19 +8184,19 @@
       <c r="V13" s="5"/>
     </row>
     <row r="14" spans="1:22" ht="33.75" customHeight="1">
-      <c r="A14" s="146"/>
-      <c r="B14" s="84"/>
-      <c r="C14" s="84"/>
-      <c r="D14" s="84"/>
-      <c r="E14" s="84"/>
-      <c r="F14" s="84"/>
-      <c r="G14" s="84"/>
-      <c r="H14" s="84"/>
-      <c r="I14" s="84"/>
-      <c r="J14" s="84"/>
-      <c r="K14" s="84"/>
-      <c r="L14" s="84"/>
-      <c r="M14" s="139"/>
+      <c r="A14" s="148"/>
+      <c r="B14" s="86"/>
+      <c r="C14" s="86"/>
+      <c r="D14" s="86"/>
+      <c r="E14" s="86"/>
+      <c r="F14" s="86"/>
+      <c r="G14" s="86"/>
+      <c r="H14" s="86"/>
+      <c r="I14" s="86"/>
+      <c r="J14" s="86"/>
+      <c r="K14" s="86"/>
+      <c r="L14" s="86"/>
+      <c r="M14" s="109"/>
       <c r="N14" s="5"/>
       <c r="O14" s="5"/>
       <c r="P14" s="5"/>
@@ -7743,19 +8208,19 @@
       <c r="V14" s="5"/>
     </row>
     <row r="15" spans="1:22" ht="33.75" customHeight="1">
-      <c r="A15" s="146"/>
-      <c r="B15" s="84"/>
-      <c r="C15" s="84"/>
-      <c r="D15" s="84"/>
-      <c r="E15" s="84"/>
-      <c r="F15" s="84"/>
-      <c r="G15" s="84"/>
-      <c r="H15" s="84"/>
-      <c r="I15" s="84"/>
-      <c r="J15" s="84"/>
-      <c r="K15" s="84"/>
-      <c r="L15" s="84"/>
-      <c r="M15" s="139"/>
+      <c r="A15" s="148"/>
+      <c r="B15" s="86"/>
+      <c r="C15" s="86"/>
+      <c r="D15" s="86"/>
+      <c r="E15" s="86"/>
+      <c r="F15" s="86"/>
+      <c r="G15" s="86"/>
+      <c r="H15" s="86"/>
+      <c r="I15" s="86"/>
+      <c r="J15" s="86"/>
+      <c r="K15" s="86"/>
+      <c r="L15" s="86"/>
+      <c r="M15" s="109"/>
       <c r="N15" s="5"/>
       <c r="O15" s="5"/>
       <c r="P15" s="5"/>
@@ -7767,19 +8232,19 @@
       <c r="V15" s="5"/>
     </row>
     <row r="16" spans="1:22" ht="33.75" customHeight="1">
-      <c r="A16" s="146"/>
-      <c r="B16" s="84"/>
-      <c r="C16" s="84"/>
-      <c r="D16" s="84"/>
-      <c r="E16" s="84"/>
-      <c r="F16" s="84"/>
-      <c r="G16" s="84"/>
-      <c r="H16" s="84"/>
-      <c r="I16" s="84"/>
-      <c r="J16" s="84"/>
-      <c r="K16" s="84"/>
-      <c r="L16" s="84"/>
-      <c r="M16" s="139"/>
+      <c r="A16" s="148"/>
+      <c r="B16" s="86"/>
+      <c r="C16" s="86"/>
+      <c r="D16" s="86"/>
+      <c r="E16" s="86"/>
+      <c r="F16" s="86"/>
+      <c r="G16" s="86"/>
+      <c r="H16" s="86"/>
+      <c r="I16" s="86"/>
+      <c r="J16" s="86"/>
+      <c r="K16" s="86"/>
+      <c r="L16" s="86"/>
+      <c r="M16" s="109"/>
       <c r="N16" s="5"/>
       <c r="O16" s="5"/>
       <c r="P16" s="5"/>
@@ -7791,19 +8256,19 @@
       <c r="V16" s="5"/>
     </row>
     <row r="17" spans="1:22" ht="33.75" customHeight="1">
-      <c r="A17" s="146"/>
-      <c r="B17" s="84"/>
-      <c r="C17" s="84"/>
-      <c r="D17" s="84"/>
-      <c r="E17" s="84"/>
-      <c r="F17" s="84"/>
-      <c r="G17" s="84"/>
-      <c r="H17" s="84"/>
-      <c r="I17" s="84"/>
-      <c r="J17" s="84"/>
-      <c r="K17" s="84"/>
-      <c r="L17" s="84"/>
-      <c r="M17" s="139"/>
+      <c r="A17" s="148"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="86"/>
+      <c r="F17" s="86"/>
+      <c r="G17" s="86"/>
+      <c r="H17" s="86"/>
+      <c r="I17" s="86"/>
+      <c r="J17" s="86"/>
+      <c r="K17" s="86"/>
+      <c r="L17" s="86"/>
+      <c r="M17" s="109"/>
       <c r="N17" s="5"/>
       <c r="O17" s="5"/>
       <c r="P17" s="5"/>
@@ -7815,19 +8280,19 @@
       <c r="V17" s="5"/>
     </row>
     <row r="18" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A18" s="146"/>
-      <c r="B18" s="84"/>
-      <c r="C18" s="84"/>
-      <c r="D18" s="84"/>
-      <c r="E18" s="84"/>
-      <c r="F18" s="84"/>
-      <c r="G18" s="84"/>
-      <c r="H18" s="84"/>
-      <c r="I18" s="84"/>
-      <c r="J18" s="84"/>
-      <c r="K18" s="84"/>
-      <c r="L18" s="84"/>
-      <c r="M18" s="139"/>
+      <c r="A18" s="148"/>
+      <c r="B18" s="86"/>
+      <c r="C18" s="86"/>
+      <c r="D18" s="86"/>
+      <c r="E18" s="86"/>
+      <c r="F18" s="86"/>
+      <c r="G18" s="86"/>
+      <c r="H18" s="86"/>
+      <c r="I18" s="86"/>
+      <c r="J18" s="86"/>
+      <c r="K18" s="86"/>
+      <c r="L18" s="86"/>
+      <c r="M18" s="109"/>
       <c r="N18" s="5"/>
       <c r="O18" s="5"/>
       <c r="P18" s="5"/>
@@ -7839,19 +8304,19 @@
       <c r="V18" s="5"/>
     </row>
     <row r="19" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A19" s="146"/>
-      <c r="B19" s="84"/>
-      <c r="C19" s="84"/>
-      <c r="D19" s="84"/>
-      <c r="E19" s="84"/>
-      <c r="F19" s="84"/>
-      <c r="G19" s="84"/>
-      <c r="H19" s="84"/>
-      <c r="I19" s="84"/>
-      <c r="J19" s="84"/>
-      <c r="K19" s="84"/>
-      <c r="L19" s="84"/>
-      <c r="M19" s="139"/>
+      <c r="A19" s="148"/>
+      <c r="B19" s="86"/>
+      <c r="C19" s="86"/>
+      <c r="D19" s="86"/>
+      <c r="E19" s="86"/>
+      <c r="F19" s="86"/>
+      <c r="G19" s="86"/>
+      <c r="H19" s="86"/>
+      <c r="I19" s="86"/>
+      <c r="J19" s="86"/>
+      <c r="K19" s="86"/>
+      <c r="L19" s="86"/>
+      <c r="M19" s="109"/>
       <c r="N19" s="5"/>
       <c r="O19" s="52"/>
       <c r="P19" s="52"/>
@@ -7863,19 +8328,19 @@
       <c r="V19" s="5"/>
     </row>
     <row r="20" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A20" s="146"/>
-      <c r="B20" s="84"/>
-      <c r="C20" s="84"/>
-      <c r="D20" s="84"/>
-      <c r="E20" s="84"/>
-      <c r="F20" s="84"/>
-      <c r="G20" s="84"/>
-      <c r="H20" s="84"/>
-      <c r="I20" s="84"/>
-      <c r="J20" s="84"/>
-      <c r="K20" s="84"/>
-      <c r="L20" s="84"/>
-      <c r="M20" s="139"/>
+      <c r="A20" s="148"/>
+      <c r="B20" s="86"/>
+      <c r="C20" s="86"/>
+      <c r="D20" s="86"/>
+      <c r="E20" s="86"/>
+      <c r="F20" s="86"/>
+      <c r="G20" s="86"/>
+      <c r="H20" s="86"/>
+      <c r="I20" s="86"/>
+      <c r="J20" s="86"/>
+      <c r="K20" s="86"/>
+      <c r="L20" s="86"/>
+      <c r="M20" s="109"/>
       <c r="N20" s="5"/>
       <c r="O20" s="52"/>
       <c r="P20" s="52"/>
@@ -7887,19 +8352,19 @@
       <c r="V20" s="5"/>
     </row>
     <row r="21" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A21" s="146"/>
-      <c r="B21" s="84"/>
-      <c r="C21" s="84"/>
-      <c r="D21" s="84"/>
-      <c r="E21" s="84"/>
-      <c r="F21" s="84"/>
-      <c r="G21" s="84"/>
-      <c r="H21" s="84"/>
-      <c r="I21" s="84"/>
-      <c r="J21" s="84"/>
-      <c r="K21" s="84"/>
-      <c r="L21" s="84"/>
-      <c r="M21" s="139"/>
+      <c r="A21" s="148"/>
+      <c r="B21" s="86"/>
+      <c r="C21" s="86"/>
+      <c r="D21" s="86"/>
+      <c r="E21" s="86"/>
+      <c r="F21" s="86"/>
+      <c r="G21" s="86"/>
+      <c r="H21" s="86"/>
+      <c r="I21" s="86"/>
+      <c r="J21" s="86"/>
+      <c r="K21" s="86"/>
+      <c r="L21" s="86"/>
+      <c r="M21" s="109"/>
       <c r="N21" s="52"/>
       <c r="O21" s="52"/>
       <c r="P21" s="52"/>
@@ -7911,19 +8376,19 @@
       <c r="V21" s="5"/>
     </row>
     <row r="22" spans="1:22" ht="22.5" customHeight="1">
-      <c r="A22" s="147"/>
-      <c r="B22" s="132"/>
-      <c r="C22" s="132"/>
-      <c r="D22" s="132"/>
-      <c r="E22" s="132"/>
-      <c r="F22" s="132"/>
-      <c r="G22" s="132"/>
-      <c r="H22" s="132"/>
-      <c r="I22" s="132"/>
-      <c r="J22" s="132"/>
-      <c r="K22" s="132"/>
-      <c r="L22" s="132"/>
-      <c r="M22" s="148"/>
+      <c r="A22" s="149"/>
+      <c r="B22" s="98"/>
+      <c r="C22" s="98"/>
+      <c r="D22" s="98"/>
+      <c r="E22" s="98"/>
+      <c r="F22" s="98"/>
+      <c r="G22" s="98"/>
+      <c r="H22" s="98"/>
+      <c r="I22" s="98"/>
+      <c r="J22" s="98"/>
+      <c r="K22" s="98"/>
+      <c r="L22" s="98"/>
+      <c r="M22" s="150"/>
       <c r="N22" s="52"/>
       <c r="O22" s="52"/>
       <c r="P22" s="52"/>
@@ -10039,4 +10504,168 @@
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U57"/>
+  <sheetViews>
+    <sheetView view="pageLayout" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="16.5"/>
+  <cols>
+    <col min="1" max="4" width="9" style="154"/>
+    <col min="5" max="5" width="12.25" style="154" customWidth="1"/>
+    <col min="6" max="16384" width="9" style="154"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" ht="98.25">
+      <c r="A1" s="160" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="160"/>
+      <c r="C1" s="160"/>
+      <c r="D1" s="160"/>
+      <c r="E1" s="160"/>
+      <c r="F1" s="160"/>
+      <c r="G1" s="160"/>
+      <c r="H1" s="160"/>
+      <c r="I1" s="160"/>
+      <c r="J1" s="160"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
+      <c r="N1" s="160"/>
+      <c r="O1" s="160"/>
+      <c r="P1" s="160"/>
+      <c r="Q1" s="160"/>
+      <c r="R1" s="160"/>
+      <c r="S1" s="160"/>
+      <c r="T1" s="160"/>
+      <c r="U1" s="160"/>
+    </row>
+    <row r="2" spans="1:21" ht="44.25" customHeight="1">
+      <c r="J2" s="152"/>
+      <c r="K2" s="153"/>
+    </row>
+    <row r="3" spans="1:21" ht="74.25">
+      <c r="A3" s="155" t="s">
+        <v>114</v>
+      </c>
+      <c r="F3" s="155" t="str">
+        <f>概要表!B3</f>
+        <v>○○分處○○站</v>
+      </c>
+      <c r="G3" s="155"/>
+    </row>
+    <row r="4" spans="1:21" ht="74.25">
+      <c r="A4" s="155" t="s">
+        <v>115</v>
+      </c>
+      <c r="F4" s="155" t="str">
+        <f>概要表!A2</f>
+        <v>○○縣市○○鄉鎮</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="74.25">
+      <c r="A5" s="155" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="74.25">
+      <c r="A6" s="155" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" ht="74.25">
+      <c r="A7" s="155" t="s">
+        <v>116</v>
+      </c>
+      <c r="F7" s="155" t="str">
+        <f>概要表!B9 &amp; "元"</f>
+        <v>0元</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" ht="74.25">
+      <c r="A8" s="155" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" ht="74.25">
+      <c r="A9" s="155" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" ht="74.25">
+      <c r="A10" s="156"/>
+    </row>
+    <row r="13" spans="1:21" ht="98.25">
+      <c r="A13" s="157" t="s">
+        <v>111</v>
+      </c>
+      <c r="B13" s="157"/>
+      <c r="C13" s="157"/>
+      <c r="D13" s="157"/>
+      <c r="E13" s="157"/>
+      <c r="F13" s="157"/>
+      <c r="G13" s="157"/>
+      <c r="H13" s="157"/>
+      <c r="I13" s="157"/>
+      <c r="J13" s="157"/>
+      <c r="K13" s="157"/>
+      <c r="L13" s="157"/>
+      <c r="M13" s="157"/>
+      <c r="N13" s="157"/>
+      <c r="O13" s="157"/>
+      <c r="P13" s="157"/>
+      <c r="Q13" s="157"/>
+      <c r="R13" s="157"/>
+      <c r="S13" s="157"/>
+      <c r="T13" s="157"/>
+      <c r="U13" s="157"/>
+    </row>
+    <row r="55" spans="1:21" ht="98.25">
+      <c r="A55" s="157" t="s">
+        <v>112</v>
+      </c>
+      <c r="B55" s="157"/>
+      <c r="C55" s="157"/>
+      <c r="D55" s="157"/>
+      <c r="E55" s="157"/>
+      <c r="F55" s="157"/>
+      <c r="G55" s="157"/>
+      <c r="H55" s="157"/>
+      <c r="I55" s="157"/>
+      <c r="J55" s="157"/>
+      <c r="K55" s="157"/>
+      <c r="L55" s="157"/>
+      <c r="M55" s="157"/>
+      <c r="N55" s="157"/>
+      <c r="O55" s="157"/>
+      <c r="P55" s="157"/>
+      <c r="Q55" s="157"/>
+      <c r="R55" s="157"/>
+      <c r="S55" s="157"/>
+      <c r="T55" s="157"/>
+      <c r="U55" s="157"/>
+    </row>
+    <row r="56" spans="1:21" ht="56.25">
+      <c r="A56" s="158"/>
+    </row>
+    <row r="57" spans="1:21">
+      <c r="A57" s="159"/>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A13:U13"/>
+    <mergeCell ref="A55:U55"/>
+    <mergeCell ref="A1:U1"/>
+  </mergeCells>
+  <phoneticPr fontId="24" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="8" orientation="landscape" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>